<commit_message>
rename form template files
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/Business Trip.xlsx
+++ b/src/main/webapp/WEB-INF/book/Business Trip.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Leave" sheetId="1" r:id="rId1"/>
+    <sheet name="Trip" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -378,6 +378,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -398,24 +416,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1029,12 +1029,12 @@
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -1059,11 +1059,11 @@
       <c r="C4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
       <c r="G4" s="6"/>
       <c r="H4" s="13" t="s">
         <v>6</v>
@@ -1096,9 +1096,9 @@
       <c r="C6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="9"/>
       <c r="H6" s="16" t="s">
         <v>7</v>
@@ -1135,9 +1135,9 @@
       <c r="C8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="7"/>
       <c r="H8" s="16" t="s">
         <v>8</v>
@@ -1181,34 +1181,34 @@
     </row>
     <row r="11" spans="2:13" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="22"/>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
       <c r="I11" s="22"/>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
       <c r="M11" s="22"/>
     </row>
     <row r="12" spans="2:13" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
       <c r="I12" s="22"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
       <c r="M12" s="22"/>
     </row>
     <row r="13" spans="2:13" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1230,10 +1230,10 @@
       <c r="C14" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="44"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="31"/>
       <c r="G14" s="31"/>
       <c r="H14" s="22"/>
@@ -1246,10 +1246,10 @@
     <row r="15" spans="2:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="22"/>
       <c r="C15" s="27"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
@@ -1260,10 +1260,10 @@
     <row r="16" spans="2:13" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="22"/>
       <c r="C16" s="30"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
@@ -1279,17 +1279,17 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" autoFilter="0"/>
   <mergeCells count="11">
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D11:H12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D16:G16"/>
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D11:H12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C23">

</xml_diff>